<commit_message>
Skipping of rows is working
</commit_message>
<xml_diff>
--- a/src/DatenMeister.Tests/Excel/Quadratzahlen.xlsx
+++ b/src/DatenMeister.Tests/Excel/Quadratzahlen.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\datenmeister-new\src\DirectUsage\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\DatenMeister\src\DatenMeister.Tests\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC8AB83-B364-4AAD-BCB3-96B4E1E427EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="22044"/>
+    <workbookView xWindow="6520" yWindow="2010" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Quadratzahl</t>
   </si>
@@ -35,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,14 +390,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -395,7 +405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -404,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -413,7 +423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -422,7 +432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -431,7 +441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -440,7 +450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -449,7 +459,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -458,7 +468,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -467,7 +477,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -476,7 +486,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -485,7 +495,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -494,7 +504,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -503,7 +513,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -512,7 +522,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -521,7 +531,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -530,7 +540,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -539,7 +549,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -548,7 +558,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -557,7 +567,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -566,7 +576,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -575,7 +585,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -584,7 +594,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -593,7 +603,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -602,7 +612,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -611,7 +621,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -620,7 +630,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -629,7 +639,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -638,7 +648,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -647,7 +657,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -656,7 +666,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -665,7 +675,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -674,7 +684,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -683,7 +693,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -692,7 +702,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -701,7 +711,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -710,7 +720,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -719,7 +729,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -728,7 +738,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -737,7 +747,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -746,7 +756,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -755,7 +765,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -764,7 +774,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -773,7 +783,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -782,7 +792,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -791,7 +801,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -800,7 +810,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -809,7 +819,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -818,11 +828,466 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
+        <f t="shared" si="0"/>
+        <v>2304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C82C587-CBBD-4F5A-9883-52D25C8AAD4D}">
+  <dimension ref="A1:B53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2*A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B53" si="0">A3*A3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>676</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>784</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>841</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>31</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>961</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>36</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>37</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>38</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>39</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>40</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>48</v>
+      </c>
+      <c r="B53">
         <f t="shared" si="0"/>
         <v>2304</v>
       </c>

</xml_diff>